<commit_message>
Adding unit tests for TemplateContextBuilder Refactoring a few things for cleanup, while I'm at it
</commit_message>
<xml_diff>
--- a/Trifolia.Test/DocSamples/ExampleTerminologyImport.xlsx
+++ b/Trifolia.Test/DocSamples/ExampleTerminologyImport.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17329"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Valuesets" sheetId="1" r:id="rId1"/>
@@ -26,15 +26,9 @@
     <t>Test Valueset 1</t>
   </si>
   <si>
-    <t>1.2.3.4</t>
-  </si>
-  <si>
     <t>Test Valueset 2</t>
   </si>
   <si>
-    <t>1.2.3.4.1</t>
-  </si>
-  <si>
     <t>Code</t>
   </si>
   <si>
@@ -59,16 +53,22 @@
     <t>TEST</t>
   </si>
   <si>
-    <t>4.3.2.1</t>
-  </si>
-  <si>
     <t>active</t>
+  </si>
+  <si>
+    <t>urn:oid:4.3.2.1</t>
+  </si>
+  <si>
+    <t>urn:oid:1.2.3.4</t>
+  </si>
+  <si>
+    <t>urn:oid:1.2.3.4.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -203,6 +203,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -238,6 +255,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -416,16 +450,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -433,20 +467,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -459,52 +493,52 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
         <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s">
-        <v>15</v>
       </c>
       <c r="F2" s="2">
         <v>41774</v>

</xml_diff>